<commit_message>
/ ‘Thesis/Microstructure/Ti-6242/Heat Treatment/Volume Fraction.xlsx’
</commit_message>
<xml_diff>
--- a/Thesis/Microstructure/Ti-6242/Heat Treatment/Volume Fraction.xlsx
+++ b/Thesis/Microstructure/Ti-6242/Heat Treatment/Volume Fraction.xlsx
@@ -24,12 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Ti6242-1.1-CS-1-(100x)</t>
   </si>
   <si>
     <t>Area of ROI (1280*1024)</t>
+  </si>
+  <si>
+    <t>Ti6242-1.1-CS-2-(100x)</t>
   </si>
 </sst>
 </file>
@@ -430,6 +433,9 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">

</xml_diff>

<commit_message>
- ‘MatLab/GrainSize.asv’ / ‘Thesis/Microstructure/Ti-6242/Heat Treatment/Volume Fraction.xlsx’
</commit_message>
<xml_diff>
--- a/Thesis/Microstructure/Ti-6242/Heat Treatment/Volume Fraction.xlsx
+++ b/Thesis/Microstructure/Ti-6242/Heat Treatment/Volume Fraction.xlsx
@@ -125,12 +125,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="S3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sharan Chandran:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Micro marker was Trimmed - 960*1280</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>Area of ROI</t>
   </si>
@@ -605,11 +629,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X356"/>
+  <dimension ref="A1:Y356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q11" sqref="Q11"/>
+      <selection pane="bottomLeft" activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,13 +647,15 @@
     <col min="14" max="14" width="12.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.140625" style="2" customWidth="1"/>
     <col min="16" max="16" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.85546875" style="2" customWidth="1"/>
-    <col min="18" max="23" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="2"/>
+    <col min="17" max="17" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" style="2" customWidth="1"/>
+    <col min="20" max="24" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -672,26 +698,26 @@
       <c r="R1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1147</v>
       </c>
@@ -724,8 +750,14 @@
       <c r="Q2" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="R2" s="1">
+        <v>635</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>587</v>
       </c>
@@ -762,8 +794,15 @@
         <f>960*1280</f>
         <v>1228800</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="R3" s="1">
+        <v>1347</v>
+      </c>
+      <c r="S3" s="4">
+        <f>960*1280</f>
+        <v>1228800</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>9364</v>
       </c>
@@ -796,8 +835,14 @@
       <c r="Q4" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="R4" s="1">
+        <v>2141</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2109</v>
       </c>
@@ -834,8 +879,15 @@
         <f>SUM(P:P)</f>
         <v>374287</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="R5" s="1">
+        <v>8090</v>
+      </c>
+      <c r="S5" s="2">
+        <f>SUM(R:R)</f>
+        <v>403130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>382</v>
       </c>
@@ -868,8 +920,14 @@
       <c r="Q6" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="R6" s="1">
+        <v>6942</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>1867</v>
       </c>
@@ -900,10 +958,18 @@
         <v>1940</v>
       </c>
       <c r="Q7" s="6">
-        <v>0.30459000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+        <f>(Q5/Q3)</f>
+        <v>0.30459554036458331</v>
+      </c>
+      <c r="R7" s="1">
+        <v>2446</v>
+      </c>
+      <c r="S7" s="6">
+        <f>(S5/S3)</f>
+        <v>0.32806803385416666</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>427</v>
       </c>
@@ -936,8 +1002,14 @@
       <c r="Q8" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="R8" s="1">
+        <v>2194</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1167</v>
       </c>
@@ -970,8 +1042,14 @@
       <c r="Q9" s="6">
         <v>9.6820000000000003E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="R9" s="1">
+        <v>4052</v>
+      </c>
+      <c r="S9" s="6">
+        <v>0.2238</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>160</v>
       </c>
@@ -995,8 +1073,12 @@
         <v>1971</v>
       </c>
       <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="R10" s="1">
+        <v>5546</v>
+      </c>
+      <c r="S10" s="1"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>413</v>
       </c>
@@ -1020,8 +1102,12 @@
         <v>305</v>
       </c>
       <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="R11" s="1">
+        <v>2724</v>
+      </c>
+      <c r="S11" s="1"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>217</v>
       </c>
@@ -1046,8 +1132,12 @@
         <v>301</v>
       </c>
       <c r="Q12" s="1"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="R12" s="1">
+        <v>4204</v>
+      </c>
+      <c r="S12" s="1"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>578</v>
       </c>
@@ -1072,8 +1162,12 @@
         <v>2241</v>
       </c>
       <c r="Q13" s="1"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="R13" s="1">
+        <v>1490</v>
+      </c>
+      <c r="S13" s="1"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>792</v>
       </c>
@@ -1098,8 +1192,12 @@
         <v>517</v>
       </c>
       <c r="Q14" s="1"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="R14" s="1">
+        <v>2848</v>
+      </c>
+      <c r="S14" s="1"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>106</v>
       </c>
@@ -1124,8 +1222,12 @@
         <v>456</v>
       </c>
       <c r="Q15" s="1"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="R15" s="1">
+        <v>14421</v>
+      </c>
+      <c r="S15" s="1"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>2003</v>
       </c>
@@ -1150,8 +1252,12 @@
         <v>416</v>
       </c>
       <c r="Q16" s="1"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16" s="1">
+        <v>11621</v>
+      </c>
+      <c r="S16" s="1"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>308</v>
       </c>
@@ -1175,8 +1281,12 @@
         <v>502</v>
       </c>
       <c r="Q17" s="1"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17" s="1">
+        <v>15959</v>
+      </c>
+      <c r="S17" s="1"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>172</v>
       </c>
@@ -1200,8 +1310,12 @@
         <v>229</v>
       </c>
       <c r="Q18" s="1"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18" s="1">
+        <v>2539</v>
+      </c>
+      <c r="S18" s="1"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>1253</v>
       </c>
@@ -1225,8 +1339,12 @@
         <v>2931</v>
       </c>
       <c r="Q19" s="1"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19" s="1">
+        <v>1143</v>
+      </c>
+      <c r="S19" s="1"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>546</v>
       </c>
@@ -1250,8 +1368,12 @@
         <v>882</v>
       </c>
       <c r="Q20" s="1"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R20" s="1">
+        <v>11192</v>
+      </c>
+      <c r="S20" s="1"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>341</v>
       </c>
@@ -1275,8 +1397,12 @@
         <v>1521</v>
       </c>
       <c r="Q21" s="1"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R21" s="1">
+        <v>3845</v>
+      </c>
+      <c r="S21" s="1"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>140</v>
       </c>
@@ -1300,8 +1426,12 @@
         <v>431</v>
       </c>
       <c r="Q22" s="1"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22" s="1">
+        <v>15697</v>
+      </c>
+      <c r="S22" s="1"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>711</v>
       </c>
@@ -1325,8 +1455,12 @@
         <v>1520</v>
       </c>
       <c r="Q23" s="1"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R23" s="1">
+        <v>1737</v>
+      </c>
+      <c r="S23" s="1"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>529</v>
       </c>
@@ -1350,8 +1484,12 @@
         <v>1014</v>
       </c>
       <c r="Q24" s="1"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R24" s="1">
+        <v>16767</v>
+      </c>
+      <c r="S24" s="1"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>400</v>
       </c>
@@ -1376,8 +1514,12 @@
         <v>435</v>
       </c>
       <c r="Q25" s="1"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R25" s="1">
+        <v>15131</v>
+      </c>
+      <c r="S25" s="1"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>215</v>
       </c>
@@ -1402,8 +1544,12 @@
         <v>263</v>
       </c>
       <c r="Q26" s="1"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R26" s="1">
+        <v>850</v>
+      </c>
+      <c r="S26" s="1"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>2959</v>
       </c>
@@ -1428,8 +1574,12 @@
         <v>971</v>
       </c>
       <c r="Q27" s="1"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R27" s="1">
+        <v>3582</v>
+      </c>
+      <c r="S27" s="1"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>349</v>
       </c>
@@ -1454,8 +1604,12 @@
         <v>503</v>
       </c>
       <c r="Q28" s="1"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R28" s="1">
+        <v>1897</v>
+      </c>
+      <c r="S28" s="1"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>972</v>
       </c>
@@ -1480,8 +1634,12 @@
         <v>7077</v>
       </c>
       <c r="Q29" s="1"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R29" s="1">
+        <v>1791</v>
+      </c>
+      <c r="S29" s="1"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>942</v>
       </c>
@@ -1506,8 +1664,12 @@
         <v>1290</v>
       </c>
       <c r="Q30" s="1"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R30" s="1">
+        <v>1357</v>
+      </c>
+      <c r="S30" s="1"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>1172</v>
       </c>
@@ -1532,8 +1694,12 @@
         <v>104</v>
       </c>
       <c r="Q31" s="1"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R31" s="1">
+        <v>2364</v>
+      </c>
+      <c r="S31" s="1"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>358</v>
       </c>
@@ -1558,8 +1724,12 @@
         <v>1067</v>
       </c>
       <c r="Q32" s="1"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R32" s="1">
+        <v>9608</v>
+      </c>
+      <c r="S32" s="1"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>2155</v>
       </c>
@@ -1584,8 +1754,12 @@
         <v>8084</v>
       </c>
       <c r="Q33" s="1"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R33" s="1">
+        <v>56145</v>
+      </c>
+      <c r="S33" s="1"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>268</v>
       </c>
@@ -1610,8 +1784,12 @@
         <v>258</v>
       </c>
       <c r="Q34" s="1"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R34" s="1">
+        <v>4266</v>
+      </c>
+      <c r="S34" s="1"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>992</v>
       </c>
@@ -1636,8 +1814,12 @@
         <v>936</v>
       </c>
       <c r="Q35" s="1"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R35" s="1">
+        <v>4119</v>
+      </c>
+      <c r="S35" s="1"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>678</v>
       </c>
@@ -1662,8 +1844,12 @@
         <v>240</v>
       </c>
       <c r="Q36" s="1"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R36" s="1">
+        <v>33922</v>
+      </c>
+      <c r="S36" s="1"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>829</v>
       </c>
@@ -1688,8 +1874,12 @@
         <v>790</v>
       </c>
       <c r="Q37" s="1"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R37" s="1">
+        <v>3771</v>
+      </c>
+      <c r="S37" s="1"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>487</v>
       </c>
@@ -1714,8 +1904,12 @@
         <v>1241</v>
       </c>
       <c r="Q38" s="1"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R38" s="1">
+        <v>2178</v>
+      </c>
+      <c r="S38" s="1"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>2772</v>
       </c>
@@ -1740,8 +1934,12 @@
         <v>1941</v>
       </c>
       <c r="Q39" s="1"/>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R39" s="1">
+        <v>989</v>
+      </c>
+      <c r="S39" s="1"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>1978</v>
       </c>
@@ -1766,8 +1964,12 @@
         <v>213</v>
       </c>
       <c r="Q40" s="1"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R40" s="1">
+        <v>4687</v>
+      </c>
+      <c r="S40" s="1"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>376</v>
       </c>
@@ -1792,8 +1994,12 @@
         <v>1338</v>
       </c>
       <c r="Q41" s="1"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R41" s="1">
+        <v>12849</v>
+      </c>
+      <c r="S41" s="1"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>205</v>
       </c>
@@ -1818,8 +2024,12 @@
         <v>231</v>
       </c>
       <c r="Q42" s="1"/>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R42" s="1">
+        <v>720</v>
+      </c>
+      <c r="S42" s="1"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>246</v>
       </c>
@@ -1844,8 +2054,12 @@
         <v>346</v>
       </c>
       <c r="Q43" s="1"/>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R43" s="1">
+        <v>6329</v>
+      </c>
+      <c r="S43" s="1"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>559</v>
       </c>
@@ -1870,8 +2084,12 @@
         <v>103</v>
       </c>
       <c r="Q44" s="1"/>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R44" s="1">
+        <v>1772</v>
+      </c>
+      <c r="S44" s="1"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>333</v>
       </c>
@@ -1896,8 +2114,12 @@
         <v>1702</v>
       </c>
       <c r="Q45" s="1"/>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R45" s="1">
+        <v>21122</v>
+      </c>
+      <c r="S45" s="1"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>588</v>
       </c>
@@ -1922,8 +2144,12 @@
         <v>2310</v>
       </c>
       <c r="Q46" s="1"/>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R46" s="1">
+        <v>3423</v>
+      </c>
+      <c r="S46" s="1"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>353</v>
       </c>
@@ -1948,8 +2174,12 @@
         <v>168</v>
       </c>
       <c r="Q47" s="1"/>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R47" s="1">
+        <v>1612</v>
+      </c>
+      <c r="S47" s="1"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>174</v>
       </c>
@@ -1974,8 +2204,12 @@
         <v>1318</v>
       </c>
       <c r="Q48" s="1"/>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R48" s="1">
+        <v>1773</v>
+      </c>
+      <c r="S48" s="1"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>1841</v>
       </c>
@@ -2000,8 +2234,12 @@
         <v>1439</v>
       </c>
       <c r="Q49" s="1"/>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R49" s="1">
+        <v>1009</v>
+      </c>
+      <c r="S49" s="1"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>674</v>
       </c>
@@ -2026,8 +2264,12 @@
         <v>970</v>
       </c>
       <c r="Q50" s="1"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R50" s="1">
+        <v>5550</v>
+      </c>
+      <c r="S50" s="1"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>1577</v>
       </c>
@@ -2052,8 +2294,12 @@
         <v>605</v>
       </c>
       <c r="Q51" s="1"/>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R51" s="1">
+        <v>30583</v>
+      </c>
+      <c r="S51" s="1"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>436</v>
       </c>
@@ -2078,8 +2324,12 @@
         <v>408</v>
       </c>
       <c r="Q52" s="1"/>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R52" s="1">
+        <v>2563</v>
+      </c>
+      <c r="S52" s="1"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>132</v>
       </c>
@@ -2104,8 +2354,12 @@
         <v>149</v>
       </c>
       <c r="Q53" s="1"/>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R53" s="1">
+        <v>9482</v>
+      </c>
+      <c r="S53" s="1"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>227</v>
       </c>
@@ -2130,8 +2384,12 @@
         <v>5041</v>
       </c>
       <c r="Q54" s="1"/>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R54" s="1">
+        <v>4134</v>
+      </c>
+      <c r="S54" s="1"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>332</v>
       </c>
@@ -2156,8 +2414,12 @@
         <v>3298</v>
       </c>
       <c r="Q55" s="1"/>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R55" s="1">
+        <v>6430</v>
+      </c>
+      <c r="S55" s="1"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>593</v>
       </c>
@@ -2182,8 +2444,12 @@
         <v>1034</v>
       </c>
       <c r="Q56" s="1"/>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R56" s="1">
+        <v>5414</v>
+      </c>
+      <c r="S56" s="1"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>359</v>
       </c>
@@ -2208,8 +2474,12 @@
         <v>208</v>
       </c>
       <c r="Q57" s="1"/>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R57" s="1">
+        <v>2128</v>
+      </c>
+      <c r="S57" s="1"/>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>369</v>
       </c>
@@ -2234,8 +2504,9 @@
         <v>335</v>
       </c>
       <c r="Q58" s="1"/>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S58" s="1"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>917</v>
       </c>
@@ -2260,8 +2531,9 @@
         <v>795</v>
       </c>
       <c r="Q59" s="1"/>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S59" s="1"/>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>1157</v>
       </c>
@@ -2286,8 +2558,9 @@
         <v>343</v>
       </c>
       <c r="Q60" s="1"/>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S60" s="1"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>217</v>
       </c>
@@ -2312,8 +2585,9 @@
         <v>2564</v>
       </c>
       <c r="Q61" s="1"/>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S61" s="1"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>378</v>
       </c>
@@ -2338,8 +2612,9 @@
         <v>376</v>
       </c>
       <c r="Q62" s="1"/>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S62" s="1"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>522</v>
       </c>
@@ -2364,8 +2639,9 @@
         <v>769</v>
       </c>
       <c r="Q63" s="1"/>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S63" s="1"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>376</v>
       </c>
@@ -2390,8 +2666,9 @@
         <v>563</v>
       </c>
       <c r="Q64" s="1"/>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S64" s="1"/>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>310</v>
       </c>
@@ -2416,8 +2693,9 @@
         <v>2965</v>
       </c>
       <c r="Q65" s="1"/>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S65" s="1"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>1307</v>
       </c>
@@ -2442,8 +2720,9 @@
         <v>520</v>
       </c>
       <c r="Q66" s="1"/>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S66" s="1"/>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>572</v>
       </c>
@@ -2468,8 +2747,9 @@
         <v>642</v>
       </c>
       <c r="Q67" s="1"/>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S67" s="1"/>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>608</v>
       </c>
@@ -2494,8 +2774,9 @@
         <v>485</v>
       </c>
       <c r="Q68" s="1"/>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S68" s="1"/>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>888</v>
       </c>
@@ -2520,8 +2801,9 @@
         <v>220</v>
       </c>
       <c r="Q69" s="1"/>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S69" s="1"/>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>1005</v>
       </c>
@@ -2546,8 +2828,9 @@
         <v>434</v>
       </c>
       <c r="Q70" s="1"/>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S70" s="1"/>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>508</v>
       </c>
@@ -2572,8 +2855,9 @@
         <v>531</v>
       </c>
       <c r="Q71" s="1"/>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S71" s="1"/>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>579</v>
       </c>
@@ -2598,8 +2882,9 @@
         <v>111</v>
       </c>
       <c r="Q72" s="1"/>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S72" s="1"/>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>3575</v>
       </c>
@@ -2624,8 +2909,9 @@
         <v>462</v>
       </c>
       <c r="Q73" s="1"/>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S73" s="1"/>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>256</v>
       </c>
@@ -2650,8 +2936,9 @@
         <v>854</v>
       </c>
       <c r="Q74" s="1"/>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S74" s="1"/>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>114</v>
       </c>
@@ -2676,8 +2963,9 @@
         <v>1558</v>
       </c>
       <c r="Q75" s="1"/>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S75" s="1"/>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>368</v>
       </c>
@@ -2702,8 +2990,9 @@
         <v>300</v>
       </c>
       <c r="Q76" s="1"/>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S76" s="1"/>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>1098</v>
       </c>
@@ -2728,8 +3017,9 @@
         <v>1701</v>
       </c>
       <c r="Q77" s="1"/>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S77" s="1"/>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>238</v>
       </c>
@@ -2754,8 +3044,9 @@
         <v>1281</v>
       </c>
       <c r="Q78" s="1"/>
-    </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S78" s="1"/>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>1355</v>
       </c>
@@ -2780,8 +3071,9 @@
         <v>2063</v>
       </c>
       <c r="Q79" s="1"/>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S79" s="1"/>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>3195</v>
       </c>
@@ -2806,8 +3098,9 @@
         <v>887</v>
       </c>
       <c r="Q80" s="1"/>
-    </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S80" s="1"/>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>825</v>
       </c>
@@ -2832,8 +3125,9 @@
         <v>1540</v>
       </c>
       <c r="Q81" s="1"/>
-    </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S81" s="1"/>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>1381</v>
       </c>
@@ -2858,8 +3152,9 @@
         <v>825</v>
       </c>
       <c r="Q82" s="1"/>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S82" s="1"/>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>141</v>
       </c>
@@ -2884,8 +3179,9 @@
         <v>814</v>
       </c>
       <c r="Q83" s="1"/>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S83" s="1"/>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>425</v>
       </c>
@@ -2910,8 +3206,9 @@
         <v>974</v>
       </c>
       <c r="Q84" s="1"/>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S84" s="1"/>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>379</v>
       </c>
@@ -2936,8 +3233,9 @@
         <v>366</v>
       </c>
       <c r="Q85" s="1"/>
-    </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S85" s="1"/>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>5634</v>
       </c>
@@ -2962,8 +3260,9 @@
         <v>180</v>
       </c>
       <c r="Q86" s="1"/>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S86" s="1"/>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>199</v>
       </c>
@@ -2988,8 +3287,9 @@
         <v>423</v>
       </c>
       <c r="Q87" s="1"/>
-    </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S87" s="1"/>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>226</v>
       </c>
@@ -3014,8 +3314,9 @@
         <v>440</v>
       </c>
       <c r="Q88" s="1"/>
-    </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S88" s="1"/>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>257</v>
       </c>
@@ -3040,8 +3341,9 @@
         <v>533</v>
       </c>
       <c r="Q89" s="1"/>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S89" s="1"/>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>2059</v>
       </c>
@@ -3066,8 +3368,9 @@
         <v>1589</v>
       </c>
       <c r="Q90" s="1"/>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S90" s="1"/>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>416</v>
       </c>
@@ -3092,8 +3395,9 @@
         <v>462</v>
       </c>
       <c r="Q91" s="1"/>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S91" s="1"/>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>152</v>
       </c>
@@ -3118,8 +3422,9 @@
         <v>570</v>
       </c>
       <c r="Q92" s="1"/>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S92" s="1"/>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>372</v>
       </c>
@@ -3144,8 +3449,9 @@
         <v>1513</v>
       </c>
       <c r="Q93" s="1"/>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S93" s="1"/>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>2275</v>
       </c>
@@ -3170,8 +3476,9 @@
         <v>267</v>
       </c>
       <c r="Q94" s="1"/>
-    </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S94" s="1"/>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>276</v>
       </c>
@@ -3196,8 +3503,9 @@
         <v>812</v>
       </c>
       <c r="Q95" s="1"/>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S95" s="1"/>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>285</v>
       </c>
@@ -3222,8 +3530,9 @@
         <v>1070</v>
       </c>
       <c r="Q96" s="1"/>
-    </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S96" s="1"/>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>338</v>
       </c>
@@ -3248,8 +3557,9 @@
         <v>499</v>
       </c>
       <c r="Q97" s="1"/>
-    </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S97" s="1"/>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>487</v>
       </c>
@@ -3274,8 +3584,9 @@
         <v>406</v>
       </c>
       <c r="Q98" s="1"/>
-    </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S98" s="1"/>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>1295</v>
       </c>
@@ -3300,8 +3611,9 @@
         <v>394</v>
       </c>
       <c r="Q99" s="1"/>
-    </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S99" s="1"/>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>425</v>
       </c>
@@ -3326,8 +3638,9 @@
         <v>246</v>
       </c>
       <c r="Q100" s="1"/>
-    </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S100" s="1"/>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>1417</v>
       </c>
@@ -3352,8 +3665,9 @@
         <v>10509</v>
       </c>
       <c r="Q101" s="1"/>
-    </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S101" s="1"/>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>509</v>
       </c>
@@ -3378,8 +3692,9 @@
         <v>545</v>
       </c>
       <c r="Q102" s="1"/>
-    </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S102" s="1"/>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>1044</v>
       </c>
@@ -3404,8 +3719,9 @@
         <v>6974</v>
       </c>
       <c r="Q103" s="1"/>
-    </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S103" s="1"/>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>1279</v>
       </c>
@@ -3430,8 +3746,9 @@
         <v>666</v>
       </c>
       <c r="Q104" s="1"/>
-    </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S104" s="1"/>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>3877</v>
       </c>
@@ -3456,8 +3773,9 @@
         <v>117</v>
       </c>
       <c r="Q105" s="1"/>
-    </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S105" s="1"/>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>589</v>
       </c>
@@ -3482,8 +3800,9 @@
         <v>338</v>
       </c>
       <c r="Q106" s="1"/>
-    </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S106" s="1"/>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>127</v>
       </c>
@@ -3508,8 +3827,9 @@
         <v>1090</v>
       </c>
       <c r="Q107" s="1"/>
-    </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S107" s="1"/>
+    </row>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>560</v>
       </c>
@@ -3534,8 +3854,9 @@
         <v>399</v>
       </c>
       <c r="Q108" s="1"/>
-    </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S108" s="1"/>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>955</v>
       </c>
@@ -3560,8 +3881,9 @@
         <v>399</v>
       </c>
       <c r="Q109" s="1"/>
-    </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S109" s="1"/>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>1736</v>
       </c>
@@ -3586,8 +3908,9 @@
         <v>901</v>
       </c>
       <c r="Q110" s="1"/>
-    </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S110" s="1"/>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>1299</v>
       </c>
@@ -3612,8 +3935,9 @@
         <v>581</v>
       </c>
       <c r="Q111" s="1"/>
-    </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S111" s="1"/>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>2793</v>
       </c>
@@ -3638,8 +3962,9 @@
         <v>3132</v>
       </c>
       <c r="Q112" s="1"/>
-    </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S112" s="1"/>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>1043</v>
       </c>
@@ -3664,8 +3989,9 @@
         <v>238</v>
       </c>
       <c r="Q113" s="1"/>
-    </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S113" s="1"/>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>279</v>
       </c>
@@ -3690,8 +4016,9 @@
         <v>2088</v>
       </c>
       <c r="Q114" s="1"/>
-    </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S114" s="1"/>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>919</v>
       </c>
@@ -3716,8 +4043,9 @@
         <v>1456</v>
       </c>
       <c r="Q115" s="1"/>
-    </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S115" s="1"/>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>1788</v>
       </c>
@@ -3742,8 +4070,9 @@
         <v>382</v>
       </c>
       <c r="Q116" s="1"/>
-    </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S116" s="1"/>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>749</v>
       </c>
@@ -3768,8 +4097,9 @@
         <v>706</v>
       </c>
       <c r="Q117" s="1"/>
-    </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S117" s="1"/>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>473</v>
       </c>
@@ -3794,8 +4124,9 @@
         <v>343</v>
       </c>
       <c r="Q118" s="1"/>
-    </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S118" s="1"/>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>967</v>
       </c>
@@ -3820,8 +4151,9 @@
         <v>199</v>
       </c>
       <c r="Q119" s="1"/>
-    </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S119" s="1"/>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>477</v>
       </c>
@@ -3846,8 +4178,9 @@
         <v>633</v>
       </c>
       <c r="Q120" s="1"/>
-    </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S120" s="1"/>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>708</v>
       </c>
@@ -3872,8 +4205,9 @@
         <v>2487</v>
       </c>
       <c r="Q121" s="1"/>
-    </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S121" s="1"/>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>404</v>
       </c>
@@ -3898,8 +4232,9 @@
         <v>1069</v>
       </c>
       <c r="Q122" s="1"/>
-    </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S122" s="1"/>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>588</v>
       </c>
@@ -3924,8 +4259,9 @@
         <v>2870</v>
       </c>
       <c r="Q123" s="1"/>
-    </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S123" s="1"/>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
         <v>208</v>
       </c>
@@ -3950,8 +4286,9 @@
         <v>149</v>
       </c>
       <c r="Q124" s="1"/>
-    </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S124" s="1"/>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>569</v>
       </c>
@@ -3976,8 +4313,9 @@
         <v>175</v>
       </c>
       <c r="Q125" s="1"/>
-    </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S125" s="1"/>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
         <v>247</v>
       </c>
@@ -4002,8 +4340,9 @@
         <v>299</v>
       </c>
       <c r="Q126" s="1"/>
-    </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S126" s="1"/>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127" s="4">
         <v>894</v>
       </c>
@@ -4028,8 +4367,9 @@
         <v>762</v>
       </c>
       <c r="Q127" s="1"/>
-    </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S127" s="1"/>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
         <v>1920</v>
       </c>
@@ -4054,8 +4394,9 @@
         <v>1173</v>
       </c>
       <c r="Q128" s="1"/>
-    </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S128" s="1"/>
+    </row>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
         <v>375</v>
       </c>
@@ -4080,8 +4421,9 @@
         <v>415</v>
       </c>
       <c r="Q129" s="1"/>
-    </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S129" s="1"/>
+    </row>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
         <v>948</v>
       </c>
@@ -4106,8 +4448,9 @@
         <v>281</v>
       </c>
       <c r="Q130" s="1"/>
-    </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S130" s="1"/>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
         <v>1303</v>
       </c>
@@ -4132,8 +4475,9 @@
         <v>2402</v>
       </c>
       <c r="Q131" s="1"/>
-    </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S131" s="1"/>
+    </row>
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
         <v>449</v>
       </c>
@@ -4158,8 +4502,9 @@
         <v>887</v>
       </c>
       <c r="Q132" s="1"/>
-    </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S132" s="1"/>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133" s="4">
         <v>1214</v>
       </c>
@@ -4184,8 +4529,9 @@
         <v>3834</v>
       </c>
       <c r="Q133" s="1"/>
-    </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S133" s="1"/>
+    </row>
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134" s="4">
         <v>348</v>
       </c>
@@ -4210,8 +4556,9 @@
         <v>658</v>
       </c>
       <c r="Q134" s="1"/>
-    </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S134" s="1"/>
+    </row>
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
         <v>511</v>
       </c>
@@ -4236,8 +4583,9 @@
         <v>639</v>
       </c>
       <c r="Q135" s="1"/>
-    </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S135" s="1"/>
+    </row>
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A136" s="4">
         <v>1490</v>
       </c>
@@ -4262,8 +4610,9 @@
         <v>447</v>
       </c>
       <c r="Q136" s="1"/>
-    </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S136" s="1"/>
+    </row>
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <v>213</v>
       </c>
@@ -4288,8 +4637,9 @@
         <v>499</v>
       </c>
       <c r="Q137" s="1"/>
-    </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S137" s="1"/>
+    </row>
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138" s="4">
         <v>810</v>
       </c>
@@ -4314,8 +4664,9 @@
         <v>246</v>
       </c>
       <c r="Q138" s="1"/>
-    </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S138" s="1"/>
+    </row>
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A139" s="4">
         <v>2612</v>
       </c>
@@ -4340,8 +4691,9 @@
         <v>644</v>
       </c>
       <c r="Q139" s="1"/>
-    </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S139" s="1"/>
+    </row>
+    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A140" s="4">
         <v>289</v>
       </c>
@@ -4366,8 +4718,9 @@
         <v>260</v>
       </c>
       <c r="Q140" s="1"/>
-    </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S140" s="1"/>
+    </row>
+    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A141" s="4">
         <v>1190</v>
       </c>
@@ -4392,8 +4745,9 @@
         <v>1488</v>
       </c>
       <c r="Q141" s="1"/>
-    </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S141" s="1"/>
+    </row>
+    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A142" s="4">
         <v>449</v>
       </c>
@@ -4418,8 +4772,9 @@
         <v>1621</v>
       </c>
       <c r="Q142" s="1"/>
-    </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S142" s="1"/>
+    </row>
+    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
         <v>444</v>
       </c>
@@ -4444,8 +4799,9 @@
         <v>323</v>
       </c>
       <c r="Q143" s="1"/>
-    </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S143" s="1"/>
+    </row>
+    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A144" s="4">
         <v>203</v>
       </c>
@@ -4470,8 +4826,9 @@
         <v>362</v>
       </c>
       <c r="Q144" s="1"/>
-    </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S144" s="1"/>
+    </row>
+    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A145" s="4">
         <v>2208</v>
       </c>
@@ -4496,8 +4853,9 @@
         <v>672</v>
       </c>
       <c r="Q145" s="1"/>
-    </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S145" s="1"/>
+    </row>
+    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A146" s="4">
         <v>695</v>
       </c>
@@ -4522,8 +4880,9 @@
         <v>499</v>
       </c>
       <c r="Q146" s="1"/>
-    </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S146" s="1"/>
+    </row>
+    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A147" s="4">
         <v>694</v>
       </c>
@@ -4548,8 +4907,9 @@
         <v>408</v>
       </c>
       <c r="Q147" s="1"/>
-    </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S147" s="1"/>
+    </row>
+    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A148" s="4">
         <v>418</v>
       </c>
@@ -4574,8 +4934,9 @@
         <v>336</v>
       </c>
       <c r="Q148" s="1"/>
-    </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S148" s="1"/>
+    </row>
+    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
         <v>250</v>
       </c>
@@ -4600,8 +4961,9 @@
         <v>139</v>
       </c>
       <c r="Q149" s="1"/>
-    </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S149" s="1"/>
+    </row>
+    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A150" s="4">
         <v>678</v>
       </c>
@@ -4626,8 +4988,9 @@
         <v>2029</v>
       </c>
       <c r="Q150" s="1"/>
-    </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S150" s="1"/>
+    </row>
+    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A151" s="4">
         <v>174</v>
       </c>
@@ -4652,8 +5015,9 @@
         <v>739</v>
       </c>
       <c r="Q151" s="1"/>
-    </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S151" s="1"/>
+    </row>
+    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A152" s="4">
         <v>359</v>
       </c>
@@ -4678,8 +5042,9 @@
         <v>469</v>
       </c>
       <c r="Q152" s="1"/>
-    </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S152" s="1"/>
+    </row>
+    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A153" s="4">
         <v>847</v>
       </c>
@@ -4704,8 +5069,9 @@
         <v>3035</v>
       </c>
       <c r="Q153" s="1"/>
-    </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S153" s="1"/>
+    </row>
+    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A154" s="4">
         <v>864</v>
       </c>
@@ -4730,8 +5096,9 @@
         <v>443</v>
       </c>
       <c r="Q154" s="1"/>
-    </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S154" s="1"/>
+    </row>
+    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A155" s="4">
         <v>1672</v>
       </c>
@@ -4756,8 +5123,9 @@
         <v>2875</v>
       </c>
       <c r="Q155" s="1"/>
-    </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S155" s="1"/>
+    </row>
+    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A156" s="4">
         <v>426</v>
       </c>
@@ -4782,8 +5150,9 @@
         <v>372</v>
       </c>
       <c r="Q156" s="1"/>
-    </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S156" s="1"/>
+    </row>
+    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A157" s="4">
         <v>1095</v>
       </c>
@@ -4808,8 +5177,9 @@
         <v>161</v>
       </c>
       <c r="Q157" s="1"/>
-    </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S157" s="1"/>
+    </row>
+    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A158" s="4">
         <v>227</v>
       </c>
@@ -4834,8 +5204,9 @@
         <v>392</v>
       </c>
       <c r="Q158" s="1"/>
-    </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S158" s="1"/>
+    </row>
+    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A159" s="4">
         <v>1271</v>
       </c>
@@ -4860,8 +5231,9 @@
         <v>534</v>
       </c>
       <c r="Q159" s="1"/>
-    </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S159" s="1"/>
+    </row>
+    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A160" s="4">
         <v>1468</v>
       </c>
@@ -4886,8 +5258,9 @@
         <v>661</v>
       </c>
       <c r="Q160" s="1"/>
-    </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S160" s="1"/>
+    </row>
+    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A161" s="4">
         <v>389</v>
       </c>
@@ -4912,8 +5285,9 @@
         <v>1024</v>
       </c>
       <c r="Q161" s="1"/>
-    </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S161" s="1"/>
+    </row>
+    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A162" s="4">
         <v>863</v>
       </c>
@@ -4938,8 +5312,9 @@
         <v>317</v>
       </c>
       <c r="Q162" s="1"/>
-    </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S162" s="1"/>
+    </row>
+    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A163" s="4">
         <v>645</v>
       </c>
@@ -4964,8 +5339,9 @@
         <v>2447</v>
       </c>
       <c r="Q163" s="1"/>
-    </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S163" s="1"/>
+    </row>
+    <row r="164" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A164" s="4">
         <v>153</v>
       </c>
@@ -4990,8 +5366,9 @@
         <v>860</v>
       </c>
       <c r="Q164" s="1"/>
-    </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S164" s="1"/>
+    </row>
+    <row r="165" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A165" s="4">
         <v>199</v>
       </c>
@@ -5016,8 +5393,9 @@
         <v>607</v>
       </c>
       <c r="Q165" s="1"/>
-    </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S165" s="1"/>
+    </row>
+    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A166" s="4">
         <v>1259</v>
       </c>
@@ -5042,8 +5420,9 @@
         <v>1516</v>
       </c>
       <c r="Q166" s="1"/>
-    </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S166" s="1"/>
+    </row>
+    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A167" s="4">
         <v>307</v>
       </c>
@@ -5068,8 +5447,9 @@
         <v>140</v>
       </c>
       <c r="Q167" s="1"/>
-    </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S167" s="1"/>
+    </row>
+    <row r="168" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A168" s="4">
         <v>634</v>
       </c>
@@ -5094,8 +5474,9 @@
         <v>927</v>
       </c>
       <c r="Q168" s="1"/>
-    </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S168" s="1"/>
+    </row>
+    <row r="169" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A169" s="4">
         <v>1174</v>
       </c>
@@ -5120,8 +5501,9 @@
         <v>635</v>
       </c>
       <c r="Q169" s="1"/>
-    </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S169" s="1"/>
+    </row>
+    <row r="170" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A170" s="4">
         <v>263</v>
       </c>
@@ -5146,8 +5528,9 @@
         <v>9051</v>
       </c>
       <c r="Q170" s="1"/>
-    </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S170" s="1"/>
+    </row>
+    <row r="171" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A171" s="4">
         <v>311</v>
       </c>
@@ -5172,8 +5555,9 @@
         <v>926</v>
       </c>
       <c r="Q171" s="1"/>
-    </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S171" s="1"/>
+    </row>
+    <row r="172" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A172" s="4">
         <v>256</v>
       </c>
@@ -5198,8 +5582,9 @@
         <v>748</v>
       </c>
       <c r="Q172" s="1"/>
-    </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S172" s="1"/>
+    </row>
+    <row r="173" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A173" s="4">
         <v>393</v>
       </c>
@@ -5224,8 +5609,9 @@
         <v>1059</v>
       </c>
       <c r="Q173" s="1"/>
-    </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S173" s="1"/>
+    </row>
+    <row r="174" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A174" s="4">
         <v>124</v>
       </c>
@@ -5250,8 +5636,9 @@
         <v>823</v>
       </c>
       <c r="Q174" s="1"/>
-    </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S174" s="1"/>
+    </row>
+    <row r="175" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A175" s="4">
         <v>1383</v>
       </c>
@@ -5276,8 +5663,9 @@
         <v>5709</v>
       </c>
       <c r="Q175" s="1"/>
-    </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S175" s="1"/>
+    </row>
+    <row r="176" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A176" s="4">
         <v>209</v>
       </c>
@@ -5302,8 +5690,9 @@
         <v>1768</v>
       </c>
       <c r="Q176" s="1"/>
-    </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S176" s="1"/>
+    </row>
+    <row r="177" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A177" s="4">
         <v>561</v>
       </c>
@@ -5328,8 +5717,9 @@
         <v>2928</v>
       </c>
       <c r="Q177" s="1"/>
-    </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S177" s="1"/>
+    </row>
+    <row r="178" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A178" s="4">
         <v>1354</v>
       </c>
@@ -5354,8 +5744,9 @@
         <v>323</v>
       </c>
       <c r="Q178" s="1"/>
-    </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S178" s="1"/>
+    </row>
+    <row r="179" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A179" s="4">
         <v>1370</v>
       </c>
@@ -5380,8 +5771,9 @@
         <v>2721</v>
       </c>
       <c r="Q179" s="1"/>
-    </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S179" s="1"/>
+    </row>
+    <row r="180" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A180" s="4">
         <v>351</v>
       </c>
@@ -5406,8 +5798,9 @@
         <v>162</v>
       </c>
       <c r="Q180" s="1"/>
-    </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S180" s="1"/>
+    </row>
+    <row r="181" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A181" s="4">
         <v>5442</v>
       </c>
@@ -5432,8 +5825,9 @@
         <v>748</v>
       </c>
       <c r="Q181" s="1"/>
-    </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S181" s="1"/>
+    </row>
+    <row r="182" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A182" s="4">
         <v>1373</v>
       </c>
@@ -5458,8 +5852,9 @@
         <v>3354</v>
       </c>
       <c r="Q182" s="1"/>
-    </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S182" s="1"/>
+    </row>
+    <row r="183" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A183" s="4">
         <v>406</v>
       </c>
@@ -5484,8 +5879,9 @@
         <v>3168</v>
       </c>
       <c r="Q183" s="1"/>
-    </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S183" s="1"/>
+    </row>
+    <row r="184" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A184" s="4">
         <v>193</v>
       </c>
@@ -5510,8 +5906,9 @@
         <v>674</v>
       </c>
       <c r="Q184" s="1"/>
-    </row>
-    <row r="185" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S184" s="1"/>
+    </row>
+    <row r="185" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A185" s="4">
         <v>408</v>
       </c>
@@ -5536,8 +5933,9 @@
         <v>870</v>
       </c>
       <c r="Q185" s="1"/>
-    </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S185" s="1"/>
+    </row>
+    <row r="186" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A186" s="4">
         <v>117</v>
       </c>
@@ -5562,8 +5960,9 @@
         <v>229</v>
       </c>
       <c r="Q186" s="1"/>
-    </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S186" s="1"/>
+    </row>
+    <row r="187" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A187" s="4">
         <v>651</v>
       </c>
@@ -5588,8 +5987,9 @@
         <v>467</v>
       </c>
       <c r="Q187" s="1"/>
-    </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S187" s="1"/>
+    </row>
+    <row r="188" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A188" s="4">
         <v>1422</v>
       </c>
@@ -5614,8 +6014,9 @@
         <v>2629</v>
       </c>
       <c r="Q188" s="1"/>
-    </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S188" s="1"/>
+    </row>
+    <row r="189" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A189" s="4">
         <v>352</v>
       </c>
@@ -5640,8 +6041,9 @@
         <v>2503</v>
       </c>
       <c r="Q189" s="1"/>
-    </row>
-    <row r="190" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S189" s="1"/>
+    </row>
+    <row r="190" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A190" s="4">
         <v>1625</v>
       </c>
@@ -5666,8 +6068,9 @@
         <v>657</v>
       </c>
       <c r="Q190" s="1"/>
-    </row>
-    <row r="191" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S190" s="1"/>
+    </row>
+    <row r="191" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A191" s="4">
         <v>324</v>
       </c>
@@ -5692,8 +6095,9 @@
         <v>685</v>
       </c>
       <c r="Q191" s="1"/>
-    </row>
-    <row r="192" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S191" s="1"/>
+    </row>
+    <row r="192" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A192" s="4">
         <v>1455</v>
       </c>
@@ -5718,8 +6122,9 @@
         <v>399</v>
       </c>
       <c r="Q192" s="1"/>
-    </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S192" s="1"/>
+    </row>
+    <row r="193" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A193" s="4">
         <v>538</v>
       </c>
@@ -5744,8 +6149,9 @@
         <v>117</v>
       </c>
       <c r="Q193" s="1"/>
-    </row>
-    <row r="194" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S193" s="1"/>
+    </row>
+    <row r="194" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A194" s="4">
         <v>345</v>
       </c>
@@ -5770,8 +6176,9 @@
         <v>195</v>
       </c>
       <c r="Q194" s="1"/>
-    </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S194" s="1"/>
+    </row>
+    <row r="195" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A195" s="4">
         <v>220</v>
       </c>
@@ -5796,8 +6203,9 @@
         <v>384</v>
       </c>
       <c r="Q195" s="1"/>
-    </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S195" s="1"/>
+    </row>
+    <row r="196" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A196" s="4">
         <v>278</v>
       </c>
@@ -5822,8 +6230,9 @@
         <v>118</v>
       </c>
       <c r="Q196" s="1"/>
-    </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S196" s="1"/>
+    </row>
+    <row r="197" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A197" s="4">
         <v>2241</v>
       </c>
@@ -5848,8 +6257,9 @@
         <v>3584</v>
       </c>
       <c r="Q197" s="1"/>
-    </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S197" s="1"/>
+    </row>
+    <row r="198" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A198" s="4">
         <v>110</v>
       </c>
@@ -5874,8 +6284,9 @@
         <v>11364</v>
       </c>
       <c r="Q198" s="1"/>
-    </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S198" s="1"/>
+    </row>
+    <row r="199" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A199" s="4">
         <v>957</v>
       </c>
@@ -5900,8 +6311,9 @@
         <v>587</v>
       </c>
       <c r="Q199" s="1"/>
-    </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S199" s="1"/>
+    </row>
+    <row r="200" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A200" s="4">
         <v>221</v>
       </c>
@@ -5926,8 +6338,9 @@
         <v>653</v>
       </c>
       <c r="Q200" s="1"/>
-    </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S200" s="1"/>
+    </row>
+    <row r="201" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A201" s="4">
         <v>194</v>
       </c>
@@ -5952,8 +6365,9 @@
         <v>625</v>
       </c>
       <c r="Q201" s="1"/>
-    </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S201" s="1"/>
+    </row>
+    <row r="202" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A202" s="4">
         <v>2117</v>
       </c>
@@ -5978,8 +6392,9 @@
         <v>376</v>
       </c>
       <c r="Q202" s="1"/>
-    </row>
-    <row r="203" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S202" s="1"/>
+    </row>
+    <row r="203" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A203" s="4">
         <v>353</v>
       </c>
@@ -6004,8 +6419,9 @@
         <v>776</v>
       </c>
       <c r="Q203" s="1"/>
-    </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S203" s="1"/>
+    </row>
+    <row r="204" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A204" s="4">
         <v>618</v>
       </c>
@@ -6030,8 +6446,9 @@
         <v>291</v>
       </c>
       <c r="Q204" s="1"/>
-    </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S204" s="1"/>
+    </row>
+    <row r="205" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A205" s="4">
         <v>1984</v>
       </c>
@@ -6056,8 +6473,9 @@
         <v>1179</v>
       </c>
       <c r="Q205" s="1"/>
-    </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S205" s="1"/>
+    </row>
+    <row r="206" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A206" s="4">
         <v>601</v>
       </c>
@@ -6082,8 +6500,9 @@
         <v>477</v>
       </c>
       <c r="Q206" s="1"/>
-    </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S206" s="1"/>
+    </row>
+    <row r="207" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A207" s="4">
         <v>365</v>
       </c>
@@ -6108,8 +6527,9 @@
         <v>1970</v>
       </c>
       <c r="Q207" s="1"/>
-    </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S207" s="1"/>
+    </row>
+    <row r="208" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A208" s="4">
         <v>2202</v>
       </c>
@@ -6134,8 +6554,9 @@
         <v>1305</v>
       </c>
       <c r="Q208" s="1"/>
-    </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S208" s="1"/>
+    </row>
+    <row r="209" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A209" s="4">
         <v>461</v>
       </c>
@@ -6160,8 +6581,9 @@
         <v>958</v>
       </c>
       <c r="Q209" s="1"/>
-    </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S209" s="1"/>
+    </row>
+    <row r="210" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A210" s="4">
         <v>166</v>
       </c>
@@ -6186,8 +6608,9 @@
         <v>349</v>
       </c>
       <c r="Q210" s="1"/>
-    </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S210" s="1"/>
+    </row>
+    <row r="211" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A211" s="4">
         <v>106</v>
       </c>
@@ -6212,8 +6635,9 @@
         <v>1596</v>
       </c>
       <c r="Q211" s="1"/>
-    </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S211" s="1"/>
+    </row>
+    <row r="212" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A212" s="4">
         <v>349</v>
       </c>
@@ -6238,8 +6662,9 @@
         <v>256</v>
       </c>
       <c r="Q212" s="1"/>
-    </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S212" s="1"/>
+    </row>
+    <row r="213" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A213" s="4">
         <v>282</v>
       </c>
@@ -6264,8 +6689,9 @@
         <v>8874</v>
       </c>
       <c r="Q213" s="1"/>
-    </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S213" s="1"/>
+    </row>
+    <row r="214" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A214" s="4">
         <v>472</v>
       </c>
@@ -6290,8 +6716,9 @@
         <v>309</v>
       </c>
       <c r="Q214" s="1"/>
-    </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S214" s="1"/>
+    </row>
+    <row r="215" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A215" s="4">
         <v>457</v>
       </c>
@@ -6316,8 +6743,9 @@
         <v>970</v>
       </c>
       <c r="Q215" s="1"/>
-    </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S215" s="1"/>
+    </row>
+    <row r="216" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A216" s="4">
         <v>2395</v>
       </c>
@@ -6342,8 +6770,9 @@
         <v>744</v>
       </c>
       <c r="Q216" s="1"/>
-    </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S216" s="1"/>
+    </row>
+    <row r="217" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A217" s="4">
         <v>813</v>
       </c>
@@ -6368,8 +6797,9 @@
         <v>130</v>
       </c>
       <c r="Q217" s="1"/>
-    </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S217" s="1"/>
+    </row>
+    <row r="218" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A218" s="4">
         <v>1681</v>
       </c>
@@ -6394,8 +6824,9 @@
         <v>862</v>
       </c>
       <c r="Q218" s="1"/>
-    </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S218" s="1"/>
+    </row>
+    <row r="219" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A219" s="4">
         <v>502</v>
       </c>
@@ -6420,8 +6851,9 @@
         <v>279</v>
       </c>
       <c r="Q219" s="1"/>
-    </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S219" s="1"/>
+    </row>
+    <row r="220" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A220" s="4">
         <v>412</v>
       </c>
@@ -6446,8 +6878,9 @@
         <v>679</v>
       </c>
       <c r="Q220" s="1"/>
-    </row>
-    <row r="221" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S220" s="1"/>
+    </row>
+    <row r="221" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A221" s="4">
         <v>1087</v>
       </c>
@@ -6472,8 +6905,9 @@
         <v>481</v>
       </c>
       <c r="Q221" s="1"/>
-    </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S221" s="1"/>
+    </row>
+    <row r="222" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A222" s="4">
         <v>1292</v>
       </c>
@@ -6498,8 +6932,9 @@
         <v>676</v>
       </c>
       <c r="Q222" s="1"/>
-    </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S222" s="1"/>
+    </row>
+    <row r="223" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A223" s="4">
         <v>2020</v>
       </c>
@@ -6524,8 +6959,9 @@
         <v>248</v>
       </c>
       <c r="Q223" s="1"/>
-    </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S223" s="1"/>
+    </row>
+    <row r="224" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A224" s="4">
         <v>225</v>
       </c>
@@ -6550,8 +6986,9 @@
         <v>190</v>
       </c>
       <c r="Q224" s="1"/>
-    </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S224" s="1"/>
+    </row>
+    <row r="225" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A225" s="4">
         <v>1638</v>
       </c>
@@ -6576,8 +7013,9 @@
         <v>115</v>
       </c>
       <c r="Q225" s="1"/>
-    </row>
-    <row r="226" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S225" s="1"/>
+    </row>
+    <row r="226" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A226" s="4">
         <v>1020</v>
       </c>
@@ -6602,8 +7040,9 @@
         <v>2972</v>
       </c>
       <c r="Q226" s="1"/>
-    </row>
-    <row r="227" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S226" s="1"/>
+    </row>
+    <row r="227" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A227" s="4">
         <v>936</v>
       </c>
@@ -6628,8 +7067,9 @@
         <v>1157</v>
       </c>
       <c r="Q227" s="1"/>
-    </row>
-    <row r="228" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S227" s="1"/>
+    </row>
+    <row r="228" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A228" s="4">
         <v>708</v>
       </c>
@@ -6654,8 +7094,9 @@
         <v>1426</v>
       </c>
       <c r="Q228" s="1"/>
-    </row>
-    <row r="229" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S228" s="1"/>
+    </row>
+    <row r="229" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A229" s="4">
         <v>261</v>
       </c>
@@ -6680,8 +7121,9 @@
         <v>1681</v>
       </c>
       <c r="Q229" s="1"/>
-    </row>
-    <row r="230" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S229" s="1"/>
+    </row>
+    <row r="230" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A230" s="4">
         <v>150</v>
       </c>
@@ -6706,8 +7148,9 @@
         <v>159</v>
       </c>
       <c r="Q230" s="1"/>
-    </row>
-    <row r="231" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S230" s="1"/>
+    </row>
+    <row r="231" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A231" s="4">
         <v>282</v>
       </c>
@@ -6732,8 +7175,9 @@
         <v>376</v>
       </c>
       <c r="Q231" s="1"/>
-    </row>
-    <row r="232" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S231" s="1"/>
+    </row>
+    <row r="232" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A232" s="4">
         <v>1313</v>
       </c>
@@ -6758,8 +7202,9 @@
         <v>2869</v>
       </c>
       <c r="Q232" s="1"/>
-    </row>
-    <row r="233" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S232" s="1"/>
+    </row>
+    <row r="233" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A233" s="4">
         <v>1603</v>
       </c>
@@ -6784,8 +7229,9 @@
         <v>3459</v>
       </c>
       <c r="Q233" s="1"/>
-    </row>
-    <row r="234" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S233" s="1"/>
+    </row>
+    <row r="234" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A234" s="4">
         <v>898</v>
       </c>
@@ -6810,8 +7256,9 @@
         <v>2791</v>
       </c>
       <c r="Q234" s="1"/>
-    </row>
-    <row r="235" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S234" s="1"/>
+    </row>
+    <row r="235" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A235" s="4">
         <v>290</v>
       </c>
@@ -6836,8 +7283,9 @@
         <v>2134</v>
       </c>
       <c r="Q235" s="1"/>
-    </row>
-    <row r="236" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S235" s="1"/>
+    </row>
+    <row r="236" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A236" s="4">
         <v>343</v>
       </c>
@@ -6862,8 +7310,9 @@
         <v>335</v>
       </c>
       <c r="Q236" s="1"/>
-    </row>
-    <row r="237" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S236" s="1"/>
+    </row>
+    <row r="237" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A237" s="4">
         <v>2031</v>
       </c>
@@ -6888,8 +7337,9 @@
         <v>311</v>
       </c>
       <c r="Q237" s="1"/>
-    </row>
-    <row r="238" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S237" s="1"/>
+    </row>
+    <row r="238" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A238" s="4">
         <v>409</v>
       </c>
@@ -6914,8 +7364,9 @@
         <v>2808</v>
       </c>
       <c r="Q238" s="1"/>
-    </row>
-    <row r="239" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S238" s="1"/>
+    </row>
+    <row r="239" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A239" s="4">
         <v>786</v>
       </c>
@@ -6940,8 +7391,9 @@
         <v>237</v>
       </c>
       <c r="Q239" s="1"/>
-    </row>
-    <row r="240" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S239" s="1"/>
+    </row>
+    <row r="240" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A240" s="4">
         <v>839</v>
       </c>
@@ -6966,8 +7418,9 @@
         <v>1583</v>
       </c>
       <c r="Q240" s="1"/>
-    </row>
-    <row r="241" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S240" s="1"/>
+    </row>
+    <row r="241" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A241" s="4">
         <v>3374</v>
       </c>
@@ -6992,8 +7445,9 @@
         <v>4088</v>
       </c>
       <c r="Q241" s="1"/>
-    </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S241" s="1"/>
+    </row>
+    <row r="242" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A242" s="4">
         <v>627</v>
       </c>
@@ -7018,8 +7472,9 @@
         <v>570</v>
       </c>
       <c r="Q242" s="1"/>
-    </row>
-    <row r="243" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S242" s="1"/>
+    </row>
+    <row r="243" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A243" s="4">
         <v>488</v>
       </c>
@@ -7044,8 +7499,9 @@
         <v>805</v>
       </c>
       <c r="Q243" s="1"/>
-    </row>
-    <row r="244" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S243" s="1"/>
+    </row>
+    <row r="244" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A244" s="4">
         <v>166</v>
       </c>
@@ -7070,8 +7526,9 @@
         <v>161</v>
       </c>
       <c r="Q244" s="1"/>
-    </row>
-    <row r="245" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S244" s="1"/>
+    </row>
+    <row r="245" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A245" s="4">
         <v>1297</v>
       </c>
@@ -7096,8 +7553,9 @@
         <v>1138</v>
       </c>
       <c r="Q245" s="1"/>
-    </row>
-    <row r="246" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S245" s="1"/>
+    </row>
+    <row r="246" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A246" s="4">
         <v>720</v>
       </c>
@@ -7122,8 +7580,9 @@
         <v>326</v>
       </c>
       <c r="Q246" s="1"/>
-    </row>
-    <row r="247" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S246" s="1"/>
+    </row>
+    <row r="247" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A247" s="4">
         <v>704</v>
       </c>
@@ -7148,8 +7607,9 @@
         <v>405</v>
       </c>
       <c r="Q247" s="1"/>
-    </row>
-    <row r="248" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S247" s="1"/>
+    </row>
+    <row r="248" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A248" s="4">
         <v>149</v>
       </c>
@@ -7174,8 +7634,9 @@
         <v>227</v>
       </c>
       <c r="Q248" s="1"/>
-    </row>
-    <row r="249" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S248" s="1"/>
+    </row>
+    <row r="249" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A249" s="4">
         <v>384</v>
       </c>
@@ -7200,8 +7661,9 @@
         <v>1066</v>
       </c>
       <c r="Q249" s="1"/>
-    </row>
-    <row r="250" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S249" s="1"/>
+    </row>
+    <row r="250" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A250" s="4">
         <v>628</v>
       </c>
@@ -7226,8 +7688,9 @@
         <v>1617</v>
       </c>
       <c r="Q250" s="1"/>
-    </row>
-    <row r="251" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S250" s="1"/>
+    </row>
+    <row r="251" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A251" s="4">
         <v>1536</v>
       </c>
@@ -7252,8 +7715,9 @@
         <v>648</v>
       </c>
       <c r="Q251" s="1"/>
-    </row>
-    <row r="252" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S251" s="1"/>
+    </row>
+    <row r="252" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A252" s="4">
         <v>1736</v>
       </c>
@@ -7278,8 +7742,9 @@
         <v>3426</v>
       </c>
       <c r="Q252" s="1"/>
-    </row>
-    <row r="253" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S252" s="1"/>
+    </row>
+    <row r="253" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A253" s="4">
         <v>2841</v>
       </c>
@@ -7304,8 +7769,9 @@
         <v>1795</v>
       </c>
       <c r="Q253" s="1"/>
-    </row>
-    <row r="254" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S253" s="1"/>
+    </row>
+    <row r="254" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A254" s="4">
         <v>132</v>
       </c>
@@ -7330,8 +7796,9 @@
         <v>5332</v>
       </c>
       <c r="Q254" s="1"/>
-    </row>
-    <row r="255" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S254" s="1"/>
+    </row>
+    <row r="255" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A255" s="4">
         <v>347</v>
       </c>
@@ -7356,8 +7823,9 @@
         <v>268</v>
       </c>
       <c r="Q255" s="1"/>
-    </row>
-    <row r="256" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S255" s="1"/>
+    </row>
+    <row r="256" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A256" s="4">
         <v>756</v>
       </c>
@@ -7382,8 +7850,9 @@
         <v>114</v>
       </c>
       <c r="Q256" s="1"/>
-    </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S256" s="1"/>
+    </row>
+    <row r="257" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A257" s="4">
         <v>519</v>
       </c>
@@ -7408,8 +7877,9 @@
         <v>2039</v>
       </c>
       <c r="Q257" s="1"/>
-    </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S257" s="1"/>
+    </row>
+    <row r="258" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A258" s="4">
         <v>298</v>
       </c>
@@ -7434,8 +7904,9 @@
         <v>2514</v>
       </c>
       <c r="Q258" s="1"/>
-    </row>
-    <row r="259" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S258" s="1"/>
+    </row>
+    <row r="259" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A259" s="4">
         <v>384</v>
       </c>
@@ -7460,8 +7931,9 @@
         <v>1341</v>
       </c>
       <c r="Q259" s="1"/>
-    </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S259" s="1"/>
+    </row>
+    <row r="260" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A260" s="4">
         <v>455</v>
       </c>
@@ -7486,8 +7958,9 @@
         <v>215</v>
       </c>
       <c r="Q260" s="1"/>
-    </row>
-    <row r="261" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S260" s="1"/>
+    </row>
+    <row r="261" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A261" s="4">
         <v>401</v>
       </c>
@@ -7512,8 +7985,9 @@
         <v>817</v>
       </c>
       <c r="Q261" s="1"/>
-    </row>
-    <row r="262" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S261" s="1"/>
+    </row>
+    <row r="262" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A262" s="4">
         <v>161</v>
       </c>
@@ -7538,8 +8012,9 @@
         <v>452</v>
       </c>
       <c r="Q262" s="1"/>
-    </row>
-    <row r="263" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S262" s="1"/>
+    </row>
+    <row r="263" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A263" s="4">
         <v>680</v>
       </c>
@@ -7564,8 +8039,9 @@
         <v>363</v>
       </c>
       <c r="Q263" s="1"/>
-    </row>
-    <row r="264" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S263" s="1"/>
+    </row>
+    <row r="264" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A264" s="4">
         <v>378</v>
       </c>
@@ -7590,8 +8066,9 @@
         <v>614</v>
       </c>
       <c r="Q264" s="1"/>
-    </row>
-    <row r="265" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S264" s="1"/>
+    </row>
+    <row r="265" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A265" s="4">
         <v>1078</v>
       </c>
@@ -7616,8 +8093,9 @@
         <v>2540</v>
       </c>
       <c r="Q265" s="1"/>
-    </row>
-    <row r="266" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S265" s="1"/>
+    </row>
+    <row r="266" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A266" s="4">
         <v>1595</v>
       </c>
@@ -7642,8 +8120,9 @@
         <v>1116</v>
       </c>
       <c r="Q266" s="1"/>
-    </row>
-    <row r="267" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S266" s="1"/>
+    </row>
+    <row r="267" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A267" s="4">
         <v>163</v>
       </c>
@@ -7668,8 +8147,9 @@
         <v>12683</v>
       </c>
       <c r="Q267" s="1"/>
-    </row>
-    <row r="268" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S267" s="1"/>
+    </row>
+    <row r="268" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A268" s="4">
         <v>291</v>
       </c>
@@ -7694,8 +8174,9 @@
         <v>633</v>
       </c>
       <c r="Q268" s="1"/>
-    </row>
-    <row r="269" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S268" s="1"/>
+    </row>
+    <row r="269" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A269" s="4">
         <v>3323</v>
       </c>
@@ -7720,8 +8201,9 @@
         <v>1293</v>
       </c>
       <c r="Q269" s="1"/>
-    </row>
-    <row r="270" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S269" s="1"/>
+    </row>
+    <row r="270" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A270" s="4">
         <v>894</v>
       </c>
@@ -7746,8 +8228,9 @@
         <v>471</v>
       </c>
       <c r="Q270" s="1"/>
-    </row>
-    <row r="271" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S270" s="1"/>
+    </row>
+    <row r="271" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A271" s="4">
         <v>245</v>
       </c>
@@ -7772,8 +8255,9 @@
         <v>1281</v>
       </c>
       <c r="Q271" s="1"/>
-    </row>
-    <row r="272" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S271" s="1"/>
+    </row>
+    <row r="272" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A272" s="4">
         <v>226</v>
       </c>
@@ -7798,8 +8282,9 @@
         <v>175</v>
       </c>
       <c r="Q272" s="1"/>
-    </row>
-    <row r="273" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S272" s="1"/>
+    </row>
+    <row r="273" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A273" s="4">
         <v>1177</v>
       </c>
@@ -7824,8 +8309,9 @@
         <v>1097</v>
       </c>
       <c r="Q273" s="1"/>
-    </row>
-    <row r="274" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S273" s="1"/>
+    </row>
+    <row r="274" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A274" s="4">
         <v>547</v>
       </c>
@@ -7850,8 +8336,9 @@
         <v>329</v>
       </c>
       <c r="Q274" s="1"/>
-    </row>
-    <row r="275" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S274" s="1"/>
+    </row>
+    <row r="275" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A275" s="4">
         <v>214</v>
       </c>
@@ -7876,8 +8363,9 @@
         <v>2550</v>
       </c>
       <c r="Q275" s="1"/>
-    </row>
-    <row r="276" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S275" s="1"/>
+    </row>
+    <row r="276" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A276" s="4">
         <v>182</v>
       </c>
@@ -7902,8 +8390,9 @@
         <v>351</v>
       </c>
       <c r="Q276" s="1"/>
-    </row>
-    <row r="277" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S276" s="1"/>
+    </row>
+    <row r="277" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A277" s="4">
         <v>2074</v>
       </c>
@@ -7928,8 +8417,9 @@
         <v>1097</v>
       </c>
       <c r="Q277" s="1"/>
-    </row>
-    <row r="278" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S277" s="1"/>
+    </row>
+    <row r="278" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A278" s="4">
         <v>307</v>
       </c>
@@ -7954,8 +8444,9 @@
         <v>759</v>
       </c>
       <c r="Q278" s="1"/>
-    </row>
-    <row r="279" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S278" s="1"/>
+    </row>
+    <row r="279" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A279" s="4">
         <v>1043</v>
       </c>
@@ -7980,8 +8471,9 @@
         <v>644</v>
       </c>
       <c r="Q279" s="1"/>
-    </row>
-    <row r="280" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S279" s="1"/>
+    </row>
+    <row r="280" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A280" s="4">
         <v>687</v>
       </c>
@@ -8006,8 +8498,9 @@
         <v>1783</v>
       </c>
       <c r="Q280" s="1"/>
-    </row>
-    <row r="281" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S280" s="1"/>
+    </row>
+    <row r="281" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A281" s="4">
         <v>718</v>
       </c>
@@ -8032,8 +8525,9 @@
         <v>1797</v>
       </c>
       <c r="Q281" s="1"/>
-    </row>
-    <row r="282" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S281" s="1"/>
+    </row>
+    <row r="282" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A282" s="4">
         <v>571</v>
       </c>
@@ -8058,8 +8552,9 @@
         <v>1446</v>
       </c>
       <c r="Q282" s="1"/>
-    </row>
-    <row r="283" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S282" s="1"/>
+    </row>
+    <row r="283" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A283" s="4">
         <v>1377</v>
       </c>
@@ -8084,8 +8579,9 @@
         <v>340</v>
       </c>
       <c r="Q283" s="1"/>
-    </row>
-    <row r="284" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S283" s="1"/>
+    </row>
+    <row r="284" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A284" s="4">
         <v>568</v>
       </c>
@@ -8110,8 +8606,9 @@
         <v>3158</v>
       </c>
       <c r="Q284" s="1"/>
-    </row>
-    <row r="285" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S284" s="1"/>
+    </row>
+    <row r="285" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A285" s="4">
         <v>1150</v>
       </c>
@@ -8136,8 +8633,9 @@
         <v>1829</v>
       </c>
       <c r="Q285" s="1"/>
-    </row>
-    <row r="286" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S285" s="1"/>
+    </row>
+    <row r="286" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A286" s="4">
         <v>170</v>
       </c>
@@ -8162,8 +8660,9 @@
         <v>713</v>
       </c>
       <c r="Q286" s="1"/>
-    </row>
-    <row r="287" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S286" s="1"/>
+    </row>
+    <row r="287" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A287" s="4">
         <v>2090</v>
       </c>
@@ -8188,8 +8687,9 @@
         <v>387</v>
       </c>
       <c r="Q287" s="1"/>
-    </row>
-    <row r="288" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S287" s="1"/>
+    </row>
+    <row r="288" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A288" s="4">
         <v>385</v>
       </c>
@@ -8214,8 +8714,9 @@
         <v>2320</v>
       </c>
       <c r="Q288" s="1"/>
-    </row>
-    <row r="289" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S288" s="1"/>
+    </row>
+    <row r="289" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A289" s="4">
         <v>505</v>
       </c>
@@ -8240,8 +8741,9 @@
         <v>400</v>
       </c>
       <c r="Q289" s="1"/>
-    </row>
-    <row r="290" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S289" s="1"/>
+    </row>
+    <row r="290" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A290" s="4">
         <v>292</v>
       </c>
@@ -8266,8 +8768,9 @@
         <v>1519</v>
       </c>
       <c r="Q290" s="1"/>
-    </row>
-    <row r="291" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S290" s="1"/>
+    </row>
+    <row r="291" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A291" s="4">
         <v>275</v>
       </c>
@@ -8292,8 +8795,9 @@
         <v>150</v>
       </c>
       <c r="Q291" s="1"/>
-    </row>
-    <row r="292" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S291" s="1"/>
+    </row>
+    <row r="292" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A292" s="4">
         <v>1209</v>
       </c>
@@ -8318,8 +8822,9 @@
         <v>872</v>
       </c>
       <c r="Q292" s="1"/>
-    </row>
-    <row r="293" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S292" s="1"/>
+    </row>
+    <row r="293" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A293" s="4">
         <v>377</v>
       </c>
@@ -8344,8 +8849,9 @@
         <v>375</v>
       </c>
       <c r="Q293" s="1"/>
-    </row>
-    <row r="294" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S293" s="1"/>
+    </row>
+    <row r="294" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A294" s="4">
         <v>477</v>
       </c>
@@ -8370,8 +8876,9 @@
         <v>603</v>
       </c>
       <c r="Q294" s="1"/>
-    </row>
-    <row r="295" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S294" s="1"/>
+    </row>
+    <row r="295" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A295" s="4">
         <v>174</v>
       </c>
@@ -8396,8 +8903,9 @@
         <v>400</v>
       </c>
       <c r="Q295" s="1"/>
-    </row>
-    <row r="296" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S295" s="1"/>
+    </row>
+    <row r="296" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A296" s="4">
         <v>240</v>
       </c>
@@ -8422,8 +8930,9 @@
         <v>861</v>
       </c>
       <c r="Q296" s="1"/>
-    </row>
-    <row r="297" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S296" s="1"/>
+    </row>
+    <row r="297" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A297" s="4">
         <v>1244</v>
       </c>
@@ -8448,8 +8957,9 @@
         <v>977</v>
       </c>
       <c r="Q297" s="1"/>
-    </row>
-    <row r="298" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S297" s="1"/>
+    </row>
+    <row r="298" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A298" s="4">
         <v>1127</v>
       </c>
@@ -8474,8 +8984,9 @@
         <v>503</v>
       </c>
       <c r="Q298" s="1"/>
-    </row>
-    <row r="299" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S298" s="1"/>
+    </row>
+    <row r="299" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A299" s="4">
         <v>2002</v>
       </c>
@@ -8500,8 +9011,9 @@
         <v>371</v>
       </c>
       <c r="Q299" s="1"/>
-    </row>
-    <row r="300" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S299" s="1"/>
+    </row>
+    <row r="300" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A300" s="4">
         <v>646</v>
       </c>
@@ -8526,8 +9038,9 @@
         <v>435</v>
       </c>
       <c r="Q300" s="1"/>
-    </row>
-    <row r="301" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S300" s="1"/>
+    </row>
+    <row r="301" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A301" s="4">
         <v>699</v>
       </c>
@@ -8552,8 +9065,9 @@
         <v>271</v>
       </c>
       <c r="Q301" s="1"/>
-    </row>
-    <row r="302" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S301" s="1"/>
+    </row>
+    <row r="302" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A302" s="4">
         <v>113</v>
       </c>
@@ -8578,8 +9092,9 @@
         <v>685</v>
       </c>
       <c r="Q302" s="1"/>
-    </row>
-    <row r="303" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S302" s="1"/>
+    </row>
+    <row r="303" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A303" s="4">
         <v>1598</v>
       </c>
@@ -8604,8 +9119,9 @@
         <v>275</v>
       </c>
       <c r="Q303" s="1"/>
-    </row>
-    <row r="304" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S303" s="1"/>
+    </row>
+    <row r="304" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A304" s="4">
         <v>206</v>
       </c>
@@ -8628,8 +9144,9 @@
         <v>417</v>
       </c>
       <c r="Q304" s="1"/>
-    </row>
-    <row r="305" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S304" s="1"/>
+    </row>
+    <row r="305" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A305" s="4">
         <v>327</v>
       </c>
@@ -8652,8 +9169,9 @@
         <v>253</v>
       </c>
       <c r="Q305" s="1"/>
-    </row>
-    <row r="306" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S305" s="1"/>
+    </row>
+    <row r="306" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A306" s="4">
         <v>966</v>
       </c>
@@ -8676,8 +9194,9 @@
         <v>338</v>
       </c>
       <c r="Q306" s="1"/>
-    </row>
-    <row r="307" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S306" s="1"/>
+    </row>
+    <row r="307" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A307" s="4">
         <v>1012</v>
       </c>
@@ -8700,8 +9219,9 @@
         <v>191</v>
       </c>
       <c r="Q307" s="1"/>
-    </row>
-    <row r="308" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S307" s="1"/>
+    </row>
+    <row r="308" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A308" s="4">
         <v>418</v>
       </c>
@@ -8721,7 +9241,7 @@
       <c r="N308" s="4"/>
       <c r="O308" s="4"/>
     </row>
-    <row r="309" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A309" s="4">
         <v>609</v>
       </c>
@@ -8741,7 +9261,7 @@
       <c r="N309" s="4"/>
       <c r="O309" s="4"/>
     </row>
-    <row r="310" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A310" s="4">
         <v>373</v>
       </c>
@@ -8761,7 +9281,7 @@
       <c r="N310" s="4"/>
       <c r="O310" s="4"/>
     </row>
-    <row r="311" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A311" s="4">
         <v>571</v>
       </c>
@@ -8781,7 +9301,7 @@
       <c r="N311" s="4"/>
       <c r="O311" s="4"/>
     </row>
-    <row r="312" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A312" s="4">
         <v>1954</v>
       </c>
@@ -8801,7 +9321,7 @@
       <c r="N312" s="4"/>
       <c r="O312" s="4"/>
     </row>
-    <row r="313" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A313" s="4">
         <v>817</v>
       </c>
@@ -8821,7 +9341,7 @@
       <c r="N313" s="4"/>
       <c r="O313" s="4"/>
     </row>
-    <row r="314" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A314" s="4">
         <v>202</v>
       </c>
@@ -8841,7 +9361,7 @@
       <c r="N314" s="4"/>
       <c r="O314" s="4"/>
     </row>
-    <row r="315" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A315" s="4">
         <v>350</v>
       </c>
@@ -8861,7 +9381,7 @@
       <c r="N315" s="4"/>
       <c r="O315" s="4"/>
     </row>
-    <row r="316" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A316" s="4">
         <v>183</v>
       </c>
@@ -8881,7 +9401,7 @@
       <c r="N316" s="4"/>
       <c r="O316" s="4"/>
     </row>
-    <row r="317" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A317" s="4">
         <v>756</v>
       </c>
@@ -8901,7 +9421,7 @@
       <c r="N317" s="4"/>
       <c r="O317" s="4"/>
     </row>
-    <row r="318" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A318" s="4">
         <v>333</v>
       </c>
@@ -8921,7 +9441,7 @@
       <c r="N318" s="4"/>
       <c r="O318" s="4"/>
     </row>
-    <row r="319" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A319" s="4">
         <v>1534</v>
       </c>
@@ -8941,7 +9461,7 @@
       <c r="N319" s="4"/>
       <c r="O319" s="4"/>
     </row>
-    <row r="320" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A320" s="4">
         <v>592</v>
       </c>

</xml_diff>